<commit_message>
initial checkin of extension
</commit_message>
<xml_diff>
--- a/MetaEdOutput/Documentation/Ed-Fi-Handbook/Ed-Fi-Handbook.xlsx
+++ b/MetaEdOutput/Documentation/Ed-Fi-Handbook/Ed-Fi-Handbook.xlsx
@@ -20344,13 +20344,13 @@
         <v/>
       </c>
       <c r="B763" t="str">
-        <v>ErrorSeverityLevel (DataValidation)</v>
+        <v>AdditionalContext (DataValidation)</v>
       </c>
       <c r="C763" t="str">
-        <v>The level of validation error</v>
+        <v>Name / Value pairs for storing data elements that do not otherwise fit into validation results.</v>
       </c>
       <c r="D763" t="str">
-        <v>Descriptor</v>
+        <v>Composite Part</v>
       </c>
       <c r="E763" t="str">
         <v/>
@@ -20359,8 +20359,11 @@
         <v/>
       </c>
       <c r="G763" t="str" xml:space="preserve">
-        <v xml:space="preserve">Used By:
-ValidationRule.ErrorSeverityLevel (as optional)</v>
+        <v xml:space="preserve">Contains:
+CustomizationValue (required)
+IdentificationCode (identity)
+Used By:
+ValidationResult.AdditionalContext (as optional collection)</v>
       </c>
     </row>
     <row r="764" xml:space="preserve">
@@ -20392,10 +20395,10 @@
         <v/>
       </c>
       <c r="B765" t="str">
-        <v>ValidationLogicType (DataValidation)</v>
+        <v>RunStatus (DataValidation)</v>
       </c>
       <c r="C765" t="str">
-        <v>The specific programing language (or pseudo-code) used to specify the rule</v>
+        <v>The status of the validation run.</v>
       </c>
       <c r="D765" t="str">
         <v>Descriptor</v>
@@ -20408,7 +20411,7 @@
       </c>
       <c r="G765" t="str" xml:space="preserve">
         <v xml:space="preserve">Used By:
-ValidationRule.ValidationLogicType (as optional)</v>
+ValidationRun.RunStatus (as required)</v>
       </c>
     </row>
     <row r="766" xml:space="preserve">
@@ -20416,10 +20419,10 @@
         <v/>
       </c>
       <c r="B766" t="str">
-        <v>ValidationRunStatus (DataValidation)</v>
+        <v>Severity (DataValidation)</v>
       </c>
       <c r="C766" t="str">
-        <v>The status of the validation run.</v>
+        <v>The level of validation error</v>
       </c>
       <c r="D766" t="str">
         <v>Descriptor</v>
@@ -20432,7 +20435,7 @@
       </c>
       <c r="G766" t="str" xml:space="preserve">
         <v xml:space="preserve">Used By:
-ValidationRun.ValidationRunStatus (as required)</v>
+ValidationRule.Severity (as optional)</v>
       </c>
     </row>
     <row r="767" xml:space="preserve">
@@ -20440,97 +20443,94 @@
         <v/>
       </c>
       <c r="B767" t="str">
+        <v>ValidationLogicType (DataValidation)</v>
+      </c>
+      <c r="C767" t="str">
+        <v>The specific programing language (or pseudo-code) used to specify the rule</v>
+      </c>
+      <c r="D767" t="str">
+        <v>Descriptor</v>
+      </c>
+      <c r="E767" t="str">
+        <v/>
+      </c>
+      <c r="F767" t="str">
+        <v/>
+      </c>
+      <c r="G767" t="str" xml:space="preserve">
+        <v xml:space="preserve">Used By:
+ValidationRule.ValidationLogicType (as optional)</v>
+      </c>
+    </row>
+    <row r="768" xml:space="preserve">
+      <c r="A768" t="str">
+        <v/>
+      </c>
+      <c r="B768" t="str">
         <v>ValidationResult (DataValidation)</v>
       </c>
-      <c r="C767" t="str">
+      <c r="C768" t="str">
         <v>A specific example of a situation that has been identified in a validation run.</v>
       </c>
-      <c r="D767" t="str">
+      <c r="D768" t="str">
         <v>Class</v>
       </c>
-      <c r="E767" t="str">
-        <v/>
-      </c>
-      <c r="F767" t="str">
-        <v/>
-      </c>
-      <c r="G767" t="str" xml:space="preserve">
+      <c r="E768" t="str">
+        <v/>
+      </c>
+      <c r="F768" t="str">
+        <v/>
+      </c>
+      <c r="G768" t="str" xml:space="preserve">
         <v xml:space="preserve">Contains:
+AdditionalContext (optional collection)
 EducationOrganization (required)
 Namespace (optional)
-OtherDetails (optional)
+ResourceId (optional)
+ResourceType (identity)
+ResultIdentifier (identity)
 Staff (optional)
 Student (optional)
-ValidationResultIdentifier (identity)
 ValidationRule (required)
 ValidationRun (optional)</v>
       </c>
     </row>
-    <row r="768" xml:space="preserve">
-      <c r="A768" t="str">
-        <v/>
-      </c>
-      <c r="B768" t="str">
+    <row r="769" xml:space="preserve">
+      <c r="A769" t="str">
+        <v/>
+      </c>
+      <c r="B769" t="str">
         <v>ValidationRule (DataValidation)</v>
       </c>
-      <c r="C768" t="str">
+      <c r="C769" t="str">
         <v>A rule that will find specific examples of invalid data.</v>
       </c>
-      <c r="D768" t="str">
+      <c r="D769" t="str">
         <v>Class</v>
       </c>
-      <c r="E768" t="str">
-        <v/>
-      </c>
-      <c r="F768" t="str">
-        <v/>
-      </c>
-      <c r="G768" t="str" xml:space="preserve">
+      <c r="E769" t="str">
+        <v/>
+      </c>
+      <c r="F769" t="str">
+        <v/>
+      </c>
+      <c r="G769" t="str" xml:space="preserve">
         <v xml:space="preserve">Contains:
 Category (optional)
 Description (optional)
-ErrorSeverityLevel (optional)
-ExternalruleCode (optional)
+ExternalRuleId (optional)
 HelpUrl (optional)
-ResourceType (optional)
 RuleIdentifier (identity)
+RuleSource (identity)
 RuleStatus (optional)
+Severity (optional)
 ShortDescription (optional)
 ValidationLogic (optional)
 ValidationLogicType (optional)
-ValidationRuleCollection (identity)
 Used By:
 ValidationResult.ValidationRule (as required)</v>
       </c>
     </row>
-    <row r="769" xml:space="preserve">
-      <c r="A769" t="str">
-        <v/>
-      </c>
-      <c r="B769" t="str">
-        <v>ValidationRuleCollection (DataValidation)</v>
-      </c>
-      <c r="C769" t="str">
-        <v>Collection of validation rule.</v>
-      </c>
-      <c r="D769" t="str">
-        <v>Class</v>
-      </c>
-      <c r="E769" t="str">
-        <v/>
-      </c>
-      <c r="F769" t="str">
-        <v/>
-      </c>
-      <c r="G769" t="str" xml:space="preserve">
-        <v xml:space="preserve">Contains:
-CollectionDescription (optional)
-CollectionIdentifier (identity)
-Used By:
-ValidationRule.ValidationRuleCollection (as identity)
-ValidationRun.ValidationRuleCollection (as identity)</v>
-      </c>
-    </row>
     <row r="770" xml:space="preserve">
       <c r="A770" t="str">
         <v/>
@@ -20552,13 +20552,12 @@
       </c>
       <c r="G770" t="str" xml:space="preserve">
         <v xml:space="preserve">Contains:
-ExaminedOds (identity)
-FinishDateTime (optional)
+Host (identity)
 RuleEngine (identity)
+RunFinishDateTime (optional)
 RunIdentifier (identity)
-StartDateTime (required)
-ValidationRuleCollection (identity)
-ValidationRunStatus (required)
+RunStartDateTime (required)
+RunStatus (required)
 Used By:
 ValidationResult.ValidationRun (as optional)</v>
       </c>
@@ -20568,17 +20567,17 @@
         <v/>
       </c>
       <c r="B771" t="str">
-        <v>ValidationResultIdentifier</v>
+        <v>CustomizationValue</v>
       </c>
       <c r="C771" t="str">
-        <v>An identifier for this validation result, unique within the validation run.</v>
+        <v>Provides the actual value of the data.</v>
       </c>
       <c r="D771" t="str">
         <v>String</v>
       </c>
       <c r="E771" t="str" xml:space="preserve">
         <v xml:space="preserve">min length: 1
-max length: 100</v>
+max length: 4000</v>
       </c>
       <c r="F771" t="str">
         <v/>
@@ -20592,17 +20591,17 @@
         <v/>
       </c>
       <c r="B772" t="str">
-        <v>OtherDetails</v>
+        <v>ResultIdentifier</v>
       </c>
       <c r="C772" t="str">
-        <v>All of the remaining details from the validation results in a JSON string.</v>
+        <v>An identifier for this validation result, unique within the validation run.</v>
       </c>
       <c r="D772" t="str">
         <v>String</v>
       </c>
       <c r="E772" t="str" xml:space="preserve">
         <v xml:space="preserve">min length: 1
-max length: 1024</v>
+max length: 100</v>
       </c>
       <c r="F772" t="str">
         <v/>
@@ -20616,10 +20615,10 @@
         <v/>
       </c>
       <c r="B773" t="str">
-        <v>RuleIdentifier</v>
+        <v>ResourceId</v>
       </c>
       <c r="C773" t="str">
-        <v>uniquely identifies a rule in a Collection</v>
+        <v>An identifier for the resource related to this validation result.</v>
       </c>
       <c r="D773" t="str">
         <v>String</v>
@@ -20640,10 +20639,10 @@
         <v/>
       </c>
       <c r="B774" t="str">
-        <v>ExternalruleCode</v>
+        <v>ResourceType</v>
       </c>
       <c r="C774" t="str">
-        <v>A reference to an external id for the rule.</v>
+        <v>Tht type of reference identified with the ReferenceId.</v>
       </c>
       <c r="D774" t="str">
         <v>String</v>
@@ -20664,10 +20663,10 @@
         <v/>
       </c>
       <c r="B775" t="str">
-        <v>ResourceType</v>
+        <v>RuleIdentifier</v>
       </c>
       <c r="C775" t="str">
-        <v>The EdFi resource type that this rule relates to (other then EducationOrganization, Student, or Staff)</v>
+        <v>uniquely identifies a rule in a Collection</v>
       </c>
       <c r="D775" t="str">
         <v>String</v>
@@ -20688,17 +20687,17 @@
         <v/>
       </c>
       <c r="B776" t="str">
-        <v>ShortDescription</v>
+        <v>RuleSource</v>
       </c>
       <c r="C776" t="str">
-        <v>This is non-structured ASCII text that will include the short details that were used in the evaluation of the validation rule.</v>
+        <v>Collection of validation rule.</v>
       </c>
       <c r="D776" t="str">
         <v>String</v>
       </c>
       <c r="E776" t="str" xml:space="preserve">
         <v xml:space="preserve">min length: 1
-max length: 1024</v>
+max length: 100</v>
       </c>
       <c r="F776" t="str">
         <v/>
@@ -20712,17 +20711,17 @@
         <v/>
       </c>
       <c r="B777" t="str">
-        <v>Category</v>
+        <v>Description</v>
       </c>
       <c r="C777" t="str">
-        <v>The category of the rule.</v>
+        <v>This is non-structured ASCII text that will include the verbose details that were used in the evaluation of the validation rule.</v>
       </c>
       <c r="D777" t="str">
         <v>String</v>
       </c>
       <c r="E777" t="str" xml:space="preserve">
         <v xml:space="preserve">min length: 1
-max length: 100</v>
+max length: 4000</v>
       </c>
       <c r="F777" t="str">
         <v/>
@@ -20736,10 +20735,10 @@
         <v/>
       </c>
       <c r="B778" t="str">
-        <v>ValidationLogic</v>
+        <v>Category</v>
       </c>
       <c r="C778" t="str">
-        <v>If applicable, the SQL statement that identifies the validation situation.</v>
+        <v>The category of the rule.</v>
       </c>
       <c r="D778" t="str">
         <v>String</v>
@@ -20760,16 +20759,16 @@
         <v/>
       </c>
       <c r="B779" t="str">
-        <v>CollectionIdentifier</v>
+        <v>ExternalRuleId</v>
       </c>
       <c r="C779" t="str">
-        <v>Rule coolection identifier.</v>
+        <v>A reference to an external id for the rule.</v>
       </c>
       <c r="D779" t="str">
         <v>String</v>
       </c>
       <c r="E779" t="str" xml:space="preserve">
-        <v xml:space="preserve">min length: 4
+        <v xml:space="preserve">min length: 1
 max length: 100</v>
       </c>
       <c r="F779" t="str">
@@ -20784,17 +20783,17 @@
         <v/>
       </c>
       <c r="B780" t="str">
-        <v>CollectionDescription</v>
+        <v>ValidationLogic</v>
       </c>
       <c r="C780" t="str">
-        <v>Rule collection description</v>
+        <v>If applicable, the SQL statement that identifies the validation situation.</v>
       </c>
       <c r="D780" t="str">
         <v>String</v>
       </c>
       <c r="E780" t="str" xml:space="preserve">
         <v xml:space="preserve">min length: 1
-max length: 255</v>
+max length: 4000</v>
       </c>
       <c r="F780" t="str">
         <v/>
@@ -20808,10 +20807,10 @@
         <v/>
       </c>
       <c r="B781" t="str">
-        <v>RuleEngine</v>
+        <v>RunIdentifier</v>
       </c>
       <c r="C781" t="str">
-        <v>A reference to the specific rules engine that ran the validation.</v>
+        <v>An identifier for the validation run that wil differentiate it from other validation runs from the same engine on the same Ods.</v>
       </c>
       <c r="D781" t="str">
         <v>String</v>
@@ -20832,7 +20831,7 @@
         <v/>
       </c>
       <c r="B782" t="str">
-        <v>ExaminedOds</v>
+        <v>Host</v>
       </c>
       <c r="C782" t="str">
         <v>A reference to the EdFi Ods that the validation egine ran agianst.</v>
@@ -20856,10 +20855,10 @@
         <v/>
       </c>
       <c r="B783" t="str">
-        <v>RunIdentifier</v>
+        <v>RuleEngine</v>
       </c>
       <c r="C783" t="str">
-        <v>An identifier for the validation run that wil differentiate it from other validation runs from the same engine on the same Ods.</v>
+        <v>A reference to the specific rules engine that ran the validation.</v>
       </c>
       <c r="D783" t="str">
         <v>String</v>

</xml_diff>